<commit_message>
working macro analysis, just finish it
</commit_message>
<xml_diff>
--- a/macro analysis/A4G2-2224.xlsx
+++ b/macro analysis/A4G2-2224.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasborn/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasborn/Desktop/analysis/ASCAM/macro analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776B0720-A5D6-2647-B8B0-9D4D390C17E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B0FFD8-A34A-A648-A071-1DB855AA3EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1160" yWindow="460" windowWidth="27540" windowHeight="20480" activeTab="8" xr2:uid="{26444931-4892-1D4A-BC65-AC3562C8D436}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27540" windowHeight="20480" activeTab="3" xr2:uid="{26444931-4892-1D4A-BC65-AC3562C8D436}"/>
   </bookViews>
   <sheets>
     <sheet name="IV" sheetId="12" r:id="rId1"/>
@@ -241,7 +241,7 @@
     <t>50Hz normalized</t>
   </si>
   <si>
-    <t>weighted tau deactivation(ms)</t>
+    <t>weighted tau (ms) decay</t>
   </si>
 </sst>
 </file>
@@ -15917,8 +15917,8 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J34" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19691,7 +19691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2ED193B-6120-524B-83D1-6B1F47AD729F}">
   <dimension ref="A1:D253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
+    <sheetView topLeftCell="A201" workbookViewId="0">
       <selection activeCell="J247" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>